<commit_message>
card details updated, testing report updated
</commit_message>
<xml_diff>
--- a/others/card_details.xlsx
+++ b/others/card_details.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\eosio_gpkbattles_contracts\others\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7899228A-7379-42B8-8719-BAAE648E2A15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56F97BE9-8808-44EF-99FD-5F5C89987ED8}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$C$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$C$26</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
   <si>
     <t>Card id</t>
   </si>
@@ -73,8 +67,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,12 +128,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -151,6 +139,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -212,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -264,7 +258,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -458,305 +452,296 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9773055-16C7-443B-89E4-2D68D6BEDFB5}">
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+    <row r="6" spans="1:8">
+      <c r="A6" s="3">
         <v>100000000007690</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+    <row r="7" spans="1:8">
+      <c r="A7" s="3">
         <v>100000000007691</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+    <row r="8" spans="1:8">
+      <c r="A8" s="3">
         <v>100000000007692</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+    <row r="9" spans="1:8">
+      <c r="A9" s="3">
         <v>100000000007693</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+    <row r="10" spans="1:8">
+      <c r="A10" s="3">
         <v>100000000007694</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3">
+        <v>100000000007695</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3">
+        <v>100000000007697</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="3">
+        <v>100000000007702</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="3">
+        <v>100000000007705</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>100000000007695</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>100000000007697</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>100000000007702</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="6" t="s">
+    <row r="15" spans="1:8">
+      <c r="A15" s="3">
+        <v>100000000007706</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="3">
+        <v>100000000007707</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3">
+        <v>100000000007710</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3">
+        <v>100000000007711</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>100000000007705</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="6" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="3">
+        <v>100000000007712</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3">
+        <v>100000000007714</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3">
+        <v>100000000007716</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3">
+        <v>100000000007720</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3">
+        <v>100000000007721</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3">
+        <v>100000000007722</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3">
+        <v>100000000007727</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>100000000007706</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="6" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="3">
+        <v>100000000007729</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>100000000007707</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>100000000007709</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>100000000007710</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>100000000007711</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>100000000007712</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>100000000007714</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>100000000007716</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>100000000007720</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>100000000007721</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>100000000007722</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>100000000007727</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>100000000007729</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:C27" xr:uid="{D089AE4A-E4E1-4F3E-8133-AD46B0D528CB}"/>
+  <autoFilter ref="A5:C26"/>
   <mergeCells count="1">
     <mergeCell ref="A1:H2"/>
   </mergeCells>

</xml_diff>